<commit_message>
plotting storage specifcially now
</commit_message>
<xml_diff>
--- a/config/plotting_config_and_timeslices-MASTER.xlsx
+++ b/config/plotting_config_and_timeslices-MASTER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\APERC\power-model\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCD5C5F-7B7B-4B3C-99E0-286C09F41619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1110ACFF-C362-4543-840C-E578AC9747BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1755" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INPUT_FUEL" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="117">
   <si>
     <t>POW_Coal_PP</t>
   </si>
@@ -374,6 +374,12 @@
   </si>
   <si>
     <t>SH2024</t>
+  </si>
+  <si>
+    <t>Storage_batt</t>
+  </si>
+  <si>
+    <t>Storage_dam</t>
   </si>
 </sst>
 </file>
@@ -504,6 +510,194 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E33DB01-6991-4D3A-4B6B-2404CE394D1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3841750" y="400050"/>
+          <a:ext cx="3060700" cy="1752600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>note that any</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> technologies not in this mapping will probably be dropped from the dataframe using </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>drop_categories_not_in_mapping() before extract_readable_name_from_mapping()</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Also, please make</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> sure any storage includes Storage at the beginnning of its name</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -849,7 +1043,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -988,7 +1182,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1073,7 +1267,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -1185,11 +1379,12 @@
         <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1198,7 +1393,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1343,8 +1538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{735169C8-9811-4ABE-A422-2C0D0CA34E87}">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1765,8 +1960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B873EB18-23BE-4A8F-8810-A9B73B0B6195}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>